<commit_message>
Segundo Caso de prueba fallo
</commit_message>
<xml_diff>
--- a/ID del Caso de prueba P1_candado.xlsx
+++ b/ID del Caso de prueba P1_candado.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Casos de pruebas\Caso de Prueba candado\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E8B7C61-32EE-4AC2-AB3E-76F581575856}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EB647FD-A393-432C-A29F-13CDA4D81ED0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{EB111D72-A51D-46D5-B50A-3BFC083371A3}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
   <si>
     <t xml:space="preserve">Ejercicio papa a paso de como abrir un canadado estando cerrado. </t>
   </si>
@@ -116,6 +116,12 @@
     <t>4. Intentar abrir el canadado levantando el arco.</t>
   </si>
   <si>
+    <t>El candado se abre sin problema y el arco se libre perfectamente.</t>
+  </si>
+  <si>
+    <t>El candado no se abre a pesar de que se ingresó la combinación correcta o se utilizó la llave adecuada.</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <b/>
@@ -135,11 +141,8 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> Exitoso  </t>
+      <t xml:space="preserve"> fallo  </t>
     </r>
-  </si>
-  <si>
-    <t>El candado se abre sin problema y el arco se libre perfectamente.</t>
   </si>
 </sst>
 </file>
@@ -293,41 +296,43 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -645,12 +650,12 @@
   <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="K21" sqref="K21"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="11.42578125" style="3"/>
+    <col min="8" max="8" width="22.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
@@ -665,242 +670,231 @@
       <c r="H1" s="14"/>
     </row>
     <row r="2" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="6"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="16"/>
+      <c r="H2" s="17"/>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B3" s="7"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="9"/>
+      <c r="B3" s="8"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="10"/>
     </row>
     <row r="4" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="8"/>
-      <c r="H4" s="9"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="10"/>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B5" s="7"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="9"/>
+      <c r="B5" s="8"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="10"/>
     </row>
     <row r="6" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="9"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="10"/>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B7" s="7"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="9"/>
+      <c r="B7" s="8"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="10"/>
     </row>
     <row r="8" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B8" s="15" t="s">
+      <c r="B8" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="C8" s="10"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="10"/>
-      <c r="G8" s="10"/>
-      <c r="H8" s="11"/>
+      <c r="C8" s="19"/>
+      <c r="D8" s="19"/>
+      <c r="E8" s="19"/>
+      <c r="F8" s="19"/>
+      <c r="G8" s="19"/>
+      <c r="H8" s="20"/>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="6"/>
+      <c r="C9" s="16"/>
+      <c r="D9" s="16"/>
+      <c r="E9" s="16"/>
+      <c r="F9" s="16"/>
+      <c r="G9" s="16"/>
+      <c r="H9" s="17"/>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="6"/>
+      <c r="C10" s="16"/>
+      <c r="D10" s="16"/>
+      <c r="E10" s="16"/>
+      <c r="F10" s="16"/>
+      <c r="G10" s="16"/>
+      <c r="H10" s="17"/>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B11" s="15" t="s">
+      <c r="B11" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5"/>
-      <c r="H11" s="6"/>
+      <c r="C11" s="16"/>
+      <c r="D11" s="16"/>
+      <c r="E11" s="16"/>
+      <c r="F11" s="16"/>
+      <c r="G11" s="16"/>
+      <c r="H11" s="17"/>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B12" s="4"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
-      <c r="H12" s="6"/>
+      <c r="B12" s="15"/>
+      <c r="C12" s="16"/>
+      <c r="D12" s="16"/>
+      <c r="E12" s="16"/>
+      <c r="F12" s="16"/>
+      <c r="G12" s="16"/>
+      <c r="H12" s="17"/>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B13" s="7" t="s">
+      <c r="B13" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C13" s="8"/>
-      <c r="D13" s="8"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="8"/>
-      <c r="G13" s="8"/>
-      <c r="H13" s="9"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="9"/>
+      <c r="H13" s="10"/>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B14" s="7" t="s">
+      <c r="B14" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
-      <c r="E14" s="8"/>
-      <c r="F14" s="8"/>
-      <c r="G14" s="8"/>
-      <c r="H14" s="9"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="9"/>
+      <c r="G14" s="9"/>
+      <c r="H14" s="10"/>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B15" s="7" t="s">
+      <c r="B15" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C15" s="8"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="8"/>
-      <c r="F15" s="8"/>
-      <c r="G15" s="8"/>
-      <c r="H15" s="9"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="9"/>
+      <c r="H15" s="10"/>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B16" s="7" t="s">
+      <c r="B16" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C16" s="8"/>
-      <c r="D16" s="8"/>
-      <c r="E16" s="8"/>
-      <c r="F16" s="8"/>
-      <c r="G16" s="8"/>
-      <c r="H16" s="9"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="9"/>
+      <c r="F16" s="9"/>
+      <c r="G16" s="9"/>
+      <c r="H16" s="10"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B17" s="2"/>
-      <c r="C17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
-      <c r="G17" s="3"/>
       <c r="H17" s="1"/>
     </row>
     <row r="18" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B18" s="16" t="s">
+      <c r="B18" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C18" s="8"/>
-      <c r="D18" s="8"/>
-      <c r="E18" s="8"/>
-      <c r="F18" s="8"/>
-      <c r="G18" s="8"/>
-      <c r="H18" s="9"/>
+      <c r="C18" s="9"/>
+      <c r="D18" s="9"/>
+      <c r="E18" s="9"/>
+      <c r="F18" s="9"/>
+      <c r="G18" s="9"/>
+      <c r="H18" s="10"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B19" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C19" s="8"/>
-      <c r="D19" s="8"/>
-      <c r="E19" s="8"/>
-      <c r="F19" s="8"/>
-      <c r="G19" s="8"/>
-      <c r="H19" s="9"/>
+      <c r="B19" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C19" s="9"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="9"/>
+      <c r="G19" s="9"/>
+      <c r="H19" s="10"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B20" s="2"/>
-      <c r="C20" s="3"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
-      <c r="G20" s="3"/>
       <c r="H20" s="1"/>
     </row>
     <row r="21" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="17"/>
-      <c r="B21" s="17" t="s">
+      <c r="A21" s="3"/>
+      <c r="B21" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C21" s="21"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="3"/>
-      <c r="G21" s="3"/>
+      <c r="C21" s="7"/>
       <c r="H21" s="1"/>
     </row>
     <row r="22" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="21"/>
-      <c r="B22" s="7"/>
-      <c r="C22" s="8"/>
-      <c r="D22" s="8"/>
-      <c r="E22" s="8"/>
-      <c r="F22" s="8"/>
-      <c r="G22" s="8"/>
-      <c r="H22" s="9"/>
+      <c r="A22" s="7"/>
+      <c r="B22" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="C22" s="22"/>
+      <c r="D22" s="22"/>
+      <c r="E22" s="22"/>
+      <c r="F22" s="22"/>
+      <c r="G22" s="22"/>
+      <c r="H22" s="23"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B23" s="2"/>
-      <c r="C23" s="3"/>
-      <c r="E23" s="3"/>
-      <c r="F23" s="3"/>
-      <c r="G23" s="3"/>
       <c r="H23" s="1"/>
     </row>
     <row r="24" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="C24" s="19"/>
-      <c r="D24" s="19"/>
-      <c r="E24" s="19"/>
-      <c r="F24" s="19"/>
-      <c r="G24" s="19"/>
-      <c r="H24" s="20"/>
+      <c r="B24" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C24" s="5"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5"/>
+      <c r="G24" s="5"/>
+      <c r="H24" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="B8:H8"/>
+    <mergeCell ref="B7:H7"/>
     <mergeCell ref="B22:H22"/>
     <mergeCell ref="B18:H18"/>
     <mergeCell ref="B19:H19"/>
@@ -917,8 +911,6 @@
     <mergeCell ref="B11:H12"/>
     <mergeCell ref="B10:H10"/>
     <mergeCell ref="B9:H9"/>
-    <mergeCell ref="B8:H8"/>
-    <mergeCell ref="B7:H7"/>
   </mergeCells>
   <conditionalFormatting sqref="B1:H20 B23:G24 A21:H21 A22:B22 H23">
     <cfRule type="iconSet" priority="2">

</xml_diff>